<commit_message>
Excluded specific countries from input and mad minor adjustments in scripts
</commit_message>
<xml_diff>
--- a/input/National_Generation_Capacities.xlsx
+++ b/input/National_Generation_Capacities.xlsx
@@ -1257,6 +1257,197 @@
 </styleSheet>
 </file>
 
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>77</xdr:col>
+      <xdr:colOff>95250</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>76199</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>77</xdr:col>
+      <xdr:colOff>1009650</xdr:colOff>
+      <xdr:row>41</xdr:row>
+      <xdr:rowOff>28574</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="2" name="Rechteck 1"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="87810975" y="1276349"/>
+          <a:ext cx="914400" cy="5514975"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent2">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent2"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent2"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" b="1"/>
+            <a:t>Values cannot be</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" b="1" baseline="0"/>
+            <a:t> provided.</a:t>
+          </a:r>
+          <a:endParaRPr lang="en-US" sz="1100" b="1"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>78</xdr:col>
+      <xdr:colOff>114300</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>66675</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>78</xdr:col>
+      <xdr:colOff>1028700</xdr:colOff>
+      <xdr:row>41</xdr:row>
+      <xdr:rowOff>19050</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="3" name="Rechteck 2"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="88944450" y="1266825"/>
+          <a:ext cx="914400" cy="5514975"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent2">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent2"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent2"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" b="1"/>
+            <a:t>Values cannot be</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" b="1" baseline="0"/>
+            <a:t> provided.</a:t>
+          </a:r>
+          <a:endParaRPr lang="en-US" sz="1100" b="1"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>114300</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>114300</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>1028700</xdr:colOff>
+      <xdr:row>41</xdr:row>
+      <xdr:rowOff>66675</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="4" name="Rechteck 3"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="16506825" y="1314450"/>
+          <a:ext cx="914400" cy="5514975"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent2">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent2"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent2"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" b="1"/>
+            <a:t>Values cannot be</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" b="1" baseline="0"/>
+            <a:t> provided.</a:t>
+          </a:r>
+          <a:endParaRPr lang="en-US" sz="1100" b="1"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
 <a:theme xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" name="Larissa">
   <a:themeElements>
@@ -1547,7 +1738,7 @@
   <dimension ref="A1:EP53"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F8" sqref="F8"/>
+      <selection activeCell="N8" sqref="N8:N44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -3742,7 +3933,7 @@
         <v>0</v>
       </c>
       <c r="N7" s="30">
-        <v>5641.2</v>
+        <v>0</v>
       </c>
       <c r="O7" s="30">
         <v>8890</v>
@@ -3934,10 +4125,10 @@
         <v>5987</v>
       </c>
       <c r="BZ7" s="30">
-        <v>5005.9369999999999</v>
+        <v>0</v>
       </c>
       <c r="CA7" s="31">
-        <v>5005.9370000000008</v>
+        <v>0</v>
       </c>
       <c r="CB7" s="31">
         <v>6300</v>
@@ -4622,7 +4813,7 @@
         <v>0</v>
       </c>
       <c r="N9" s="24">
-        <v>470</v>
+        <v>0</v>
       </c>
       <c r="O9" s="24">
         <v>670</v>
@@ -4814,10 +5005,10 @@
         <v>0</v>
       </c>
       <c r="BZ9" s="17">
-        <v>220</v>
+        <v>0</v>
       </c>
       <c r="CA9" s="34">
-        <v>220</v>
+        <v>0</v>
       </c>
       <c r="CB9" s="34">
         <v>440</v>
@@ -5062,7 +5253,7 @@
         <v>0</v>
       </c>
       <c r="N10" s="24">
-        <v>224.19999999999996</v>
+        <v>0</v>
       </c>
       <c r="O10" s="24">
         <v>370</v>
@@ -5502,7 +5693,7 @@
         <v>0</v>
       </c>
       <c r="N11" s="24">
-        <v>4632</v>
+        <v>0</v>
       </c>
       <c r="O11" s="24">
         <v>7850</v>
@@ -5694,10 +5885,10 @@
         <v>0</v>
       </c>
       <c r="BZ11" s="17">
-        <v>2586.7000000000003</v>
+        <v>0</v>
       </c>
       <c r="CA11" s="34">
-        <v>2586.7000000000003</v>
+        <v>0</v>
       </c>
       <c r="CB11" s="34">
         <v>4560</v>
@@ -5942,7 +6133,7 @@
         <v>0</v>
       </c>
       <c r="N12" s="24">
-        <v>3489</v>
+        <v>0</v>
       </c>
       <c r="O12" s="24">
         <v>0</v>
@@ -6134,10 +6325,10 @@
         <v>0</v>
       </c>
       <c r="BZ12" s="17">
-        <v>587.1</v>
+        <v>0</v>
       </c>
       <c r="CA12" s="34">
-        <v>587.1</v>
+        <v>0</v>
       </c>
       <c r="CB12" s="34">
         <v>0</v>
@@ -6382,7 +6573,7 @@
         <v>0</v>
       </c>
       <c r="N13" s="24">
-        <v>292</v>
+        <v>0</v>
       </c>
       <c r="O13" s="24">
         <v>0</v>
@@ -6574,10 +6765,10 @@
         <v>0</v>
       </c>
       <c r="BZ13" s="17">
-        <v>1999.6000000000001</v>
+        <v>0</v>
       </c>
       <c r="CA13" s="34">
-        <v>1999.6000000000001</v>
+        <v>0</v>
       </c>
       <c r="CB13" s="34">
         <v>0</v>
@@ -6822,7 +7013,7 @@
         <v>0</v>
       </c>
       <c r="N14" s="24">
-        <v>851</v>
+        <v>0</v>
       </c>
       <c r="O14" s="24">
         <v>0</v>
@@ -8142,7 +8333,7 @@
         <v>0</v>
       </c>
       <c r="N17" s="24">
-        <v>315</v>
+        <v>0</v>
       </c>
       <c r="O17" s="24">
         <v>0</v>
@@ -9214,10 +9405,10 @@
         <v>5987</v>
       </c>
       <c r="BZ19" s="17">
-        <v>2199.2370000000001</v>
+        <v>0</v>
       </c>
       <c r="CA19" s="17">
-        <v>2199.2370000000005</v>
+        <v>0</v>
       </c>
       <c r="CB19" s="17">
         <v>0</v>
@@ -9462,7 +9653,7 @@
         <v>0</v>
       </c>
       <c r="N20" s="43">
-        <v>5925.8</v>
+        <v>0</v>
       </c>
       <c r="O20" s="43">
         <v>3910</v>
@@ -9654,10 +9845,10 @@
         <v>2000</v>
       </c>
       <c r="BZ20" s="43">
-        <v>2000</v>
+        <v>0</v>
       </c>
       <c r="CA20" s="44">
-        <v>2000</v>
+        <v>0</v>
       </c>
       <c r="CB20" s="44">
         <v>1900</v>
@@ -9902,7 +10093,7 @@
         <v>0</v>
       </c>
       <c r="N21" s="48">
-        <v>2974.2</v>
+        <v>0</v>
       </c>
       <c r="O21" s="48">
         <v>7040</v>
@@ -10094,10 +10285,10 @@
         <v>421</v>
       </c>
       <c r="BZ21" s="48">
-        <v>286.5</v>
+        <v>0</v>
       </c>
       <c r="CA21" s="49">
-        <v>316.5</v>
+        <v>0</v>
       </c>
       <c r="CB21" s="49">
         <v>850.00000000000011</v>
@@ -10342,7 +10533,7 @@
         <v>0</v>
       </c>
       <c r="N22" s="24">
-        <v>1394.1000000000001</v>
+        <v>0</v>
       </c>
       <c r="O22" s="24">
         <v>1430</v>
@@ -12982,7 +13173,7 @@
         <v>0</v>
       </c>
       <c r="N28" s="24">
-        <v>1394.1000000000001</v>
+        <v>0</v>
       </c>
       <c r="O28" s="24">
         <v>1430</v>
@@ -13422,7 +13613,7 @@
         <v>0</v>
       </c>
       <c r="N29" s="24">
-        <v>900.30000000000007</v>
+        <v>0</v>
       </c>
       <c r="O29" s="24">
         <v>1890</v>
@@ -13614,10 +13805,10 @@
         <v>329</v>
       </c>
       <c r="BZ29" s="17">
-        <v>48</v>
+        <v>0</v>
       </c>
       <c r="CA29" s="34">
-        <v>48</v>
+        <v>0</v>
       </c>
       <c r="CB29" s="34">
         <v>330</v>
@@ -14054,10 +14245,10 @@
         <v>329</v>
       </c>
       <c r="BZ30" s="17">
-        <v>48</v>
+        <v>0</v>
       </c>
       <c r="CA30" s="34">
-        <v>48</v>
+        <v>0</v>
       </c>
       <c r="CB30" s="34">
         <v>330</v>
@@ -14742,7 +14933,7 @@
         <v>0</v>
       </c>
       <c r="N32" s="24">
-        <v>900.30000000000007</v>
+        <v>0</v>
       </c>
       <c r="O32" s="24">
         <v>0</v>
@@ -17822,7 +18013,7 @@
         <v>0</v>
       </c>
       <c r="N39" s="24">
-        <v>679.8</v>
+        <v>0</v>
       </c>
       <c r="O39" s="24">
         <v>1290</v>
@@ -18014,10 +18205,10 @@
         <v>0</v>
       </c>
       <c r="BZ39" s="17">
-        <v>238.5</v>
+        <v>0</v>
       </c>
       <c r="CA39" s="34">
-        <v>268.5</v>
+        <v>0</v>
       </c>
       <c r="CB39" s="34">
         <v>470</v>
@@ -18454,10 +18645,10 @@
         <v>0</v>
       </c>
       <c r="BZ40" s="17">
-        <v>238.5</v>
+        <v>0</v>
       </c>
       <c r="CA40" s="34">
-        <v>268.5</v>
+        <v>0</v>
       </c>
       <c r="CB40" s="34">
         <v>470</v>
@@ -19142,7 +19333,7 @@
         <v>0</v>
       </c>
       <c r="N42" s="24">
-        <v>679.8</v>
+        <v>0</v>
       </c>
       <c r="O42" s="24">
         <v>0</v>
@@ -19774,10 +19965,10 @@
         <v>0</v>
       </c>
       <c r="BZ43" s="59">
-        <v>1090</v>
+        <v>0</v>
       </c>
       <c r="CA43" s="59">
-        <v>1090</v>
+        <v>0</v>
       </c>
       <c r="CB43" s="59">
         <v>0</v>
@@ -20022,7 +20213,7 @@
         <v>0</v>
       </c>
       <c r="N44" s="67">
-        <v>14541.2</v>
+        <v>0</v>
       </c>
       <c r="O44" s="67">
         <v>19840</v>
@@ -20214,10 +20405,10 @@
         <v>8408</v>
       </c>
       <c r="BZ44" s="64">
-        <v>8382.4369999999999</v>
+        <v>0</v>
       </c>
       <c r="CA44" s="65">
-        <v>8412.4370000000017</v>
+        <v>0</v>
       </c>
       <c r="CB44" s="65">
         <v>9050</v>
@@ -20591,5 +20782,6 @@
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Adjusted input data for Germany
</commit_message>
<xml_diff>
--- a/input/National_Generation_Capacities.xlsx
+++ b/input/National_Generation_Capacities.xlsx
@@ -1186,6 +1186,42 @@
     <xf numFmtId="0" fontId="5" fillId="8" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="8" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="8" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="8" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left" vertical="top" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="2" fillId="8" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1197,42 +1233,6 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="2" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="8" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="8" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="5" fillId="8" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="2">
@@ -1404,6 +1404,130 @@
       <xdr:spPr>
         <a:xfrm>
           <a:off x="16506825" y="1314450"/>
+          <a:ext cx="914400" cy="5514975"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent2">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent2"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent2"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" b="1"/>
+            <a:t>Values cannot be</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" b="1" baseline="0"/>
+            <a:t> provided.</a:t>
+          </a:r>
+          <a:endParaRPr lang="en-US" sz="1100" b="1"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>32</xdr:col>
+      <xdr:colOff>85725</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>66675</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>32</xdr:col>
+      <xdr:colOff>1000125</xdr:colOff>
+      <xdr:row>41</xdr:row>
+      <xdr:rowOff>19050</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="5" name="Rechteck 4"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="37652325" y="1266825"/>
+          <a:ext cx="914400" cy="5514975"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="2">
+          <a:schemeClr val="accent2">
+            <a:shade val="50000"/>
+          </a:schemeClr>
+        </a:lnRef>
+        <a:fillRef idx="1">
+          <a:schemeClr val="accent2"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:schemeClr val="accent2"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="lt1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" rtlCol="0" anchor="ctr"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr algn="ctr"/>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" b="1"/>
+            <a:t>Values cannot be</a:t>
+          </a:r>
+          <a:r>
+            <a:rPr lang="en-US" sz="1100" b="1" baseline="0"/>
+            <a:t> provided.</a:t>
+          </a:r>
+          <a:endParaRPr lang="en-US" sz="1100" b="1"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>33</xdr:col>
+      <xdr:colOff>104775</xdr:colOff>
+      <xdr:row>7</xdr:row>
+      <xdr:rowOff>76200</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>33</xdr:col>
+      <xdr:colOff>1019175</xdr:colOff>
+      <xdr:row>41</xdr:row>
+      <xdr:rowOff>28575</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="6" name="Rechteck 5"/>
+        <xdr:cNvSpPr/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="38785800" y="1276350"/>
           <a:ext cx="914400" cy="5514975"/>
         </a:xfrm>
         <a:prstGeom prst="rect">
@@ -1737,8 +1861,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:EP53"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="N8" sqref="N8:N44"/>
+    <sheetView tabSelected="1" topLeftCell="AB1" workbookViewId="0">
+      <selection activeCell="AG7" sqref="AG7:AH44"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -1752,213 +1876,213 @@
   <sheetData>
     <row r="1" spans="1:146" s="75" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="68"/>
-      <c r="B1" s="119" t="s">
+      <c r="B1" s="131" t="s">
         <v>116</v>
       </c>
-      <c r="C1" s="120"/>
-      <c r="D1" s="120"/>
-      <c r="E1" s="120"/>
-      <c r="F1" s="121"/>
-      <c r="G1" s="123" t="s">
-        <v>0</v>
-      </c>
-      <c r="H1" s="124"/>
-      <c r="I1" s="124"/>
-      <c r="J1" s="124"/>
-      <c r="K1" s="125"/>
-      <c r="L1" s="123" t="s">
+      <c r="C1" s="132"/>
+      <c r="D1" s="132"/>
+      <c r="E1" s="132"/>
+      <c r="F1" s="133"/>
+      <c r="G1" s="119" t="s">
+        <v>0</v>
+      </c>
+      <c r="H1" s="120"/>
+      <c r="I1" s="120"/>
+      <c r="J1" s="120"/>
+      <c r="K1" s="121"/>
+      <c r="L1" s="119" t="s">
         <v>1</v>
       </c>
-      <c r="M1" s="124"/>
-      <c r="N1" s="124"/>
-      <c r="O1" s="124"/>
-      <c r="P1" s="125"/>
-      <c r="Q1" s="123" t="s">
+      <c r="M1" s="120"/>
+      <c r="N1" s="120"/>
+      <c r="O1" s="120"/>
+      <c r="P1" s="121"/>
+      <c r="Q1" s="119" t="s">
         <v>53</v>
       </c>
-      <c r="R1" s="124"/>
-      <c r="S1" s="124"/>
-      <c r="T1" s="124"/>
-      <c r="U1" s="125"/>
-      <c r="V1" s="123" t="s">
+      <c r="R1" s="120"/>
+      <c r="S1" s="120"/>
+      <c r="T1" s="120"/>
+      <c r="U1" s="121"/>
+      <c r="V1" s="119" t="s">
         <v>2</v>
       </c>
-      <c r="W1" s="124"/>
-      <c r="X1" s="124"/>
-      <c r="Y1" s="124"/>
-      <c r="Z1" s="125"/>
-      <c r="AA1" s="123" t="s">
+      <c r="W1" s="120"/>
+      <c r="X1" s="120"/>
+      <c r="Y1" s="120"/>
+      <c r="Z1" s="121"/>
+      <c r="AA1" s="119" t="s">
         <v>3</v>
       </c>
-      <c r="AB1" s="124"/>
-      <c r="AC1" s="124"/>
-      <c r="AD1" s="124"/>
-      <c r="AE1" s="125"/>
-      <c r="AF1" s="123" t="s">
+      <c r="AB1" s="120"/>
+      <c r="AC1" s="120"/>
+      <c r="AD1" s="120"/>
+      <c r="AE1" s="121"/>
+      <c r="AF1" s="119" t="s">
         <v>4</v>
       </c>
-      <c r="AG1" s="124"/>
-      <c r="AH1" s="124"/>
-      <c r="AI1" s="124"/>
-      <c r="AJ1" s="125"/>
-      <c r="AK1" s="123" t="s">
+      <c r="AG1" s="120"/>
+      <c r="AH1" s="120"/>
+      <c r="AI1" s="120"/>
+      <c r="AJ1" s="121"/>
+      <c r="AK1" s="119" t="s">
         <v>5</v>
       </c>
-      <c r="AL1" s="124"/>
-      <c r="AM1" s="124"/>
-      <c r="AN1" s="124"/>
-      <c r="AO1" s="125"/>
-      <c r="AP1" s="123" t="s">
+      <c r="AL1" s="120"/>
+      <c r="AM1" s="120"/>
+      <c r="AN1" s="120"/>
+      <c r="AO1" s="121"/>
+      <c r="AP1" s="119" t="s">
         <v>54</v>
       </c>
-      <c r="AQ1" s="124"/>
-      <c r="AR1" s="124"/>
-      <c r="AS1" s="124"/>
-      <c r="AT1" s="125"/>
-      <c r="AU1" s="123" t="s">
+      <c r="AQ1" s="120"/>
+      <c r="AR1" s="120"/>
+      <c r="AS1" s="120"/>
+      <c r="AT1" s="121"/>
+      <c r="AU1" s="119" t="s">
         <v>6</v>
       </c>
-      <c r="AV1" s="124"/>
-      <c r="AW1" s="124"/>
-      <c r="AX1" s="124"/>
-      <c r="AY1" s="125"/>
-      <c r="AZ1" s="123" t="s">
+      <c r="AV1" s="120"/>
+      <c r="AW1" s="120"/>
+      <c r="AX1" s="120"/>
+      <c r="AY1" s="121"/>
+      <c r="AZ1" s="119" t="s">
         <v>7</v>
       </c>
-      <c r="BA1" s="124"/>
-      <c r="BB1" s="124"/>
-      <c r="BC1" s="124"/>
-      <c r="BD1" s="125"/>
-      <c r="BE1" s="123" t="s">
+      <c r="BA1" s="120"/>
+      <c r="BB1" s="120"/>
+      <c r="BC1" s="120"/>
+      <c r="BD1" s="121"/>
+      <c r="BE1" s="119" t="s">
         <v>55</v>
       </c>
-      <c r="BF1" s="124"/>
-      <c r="BG1" s="124"/>
-      <c r="BH1" s="124"/>
-      <c r="BI1" s="125"/>
-      <c r="BJ1" s="123" t="s">
+      <c r="BF1" s="120"/>
+      <c r="BG1" s="120"/>
+      <c r="BH1" s="120"/>
+      <c r="BI1" s="121"/>
+      <c r="BJ1" s="119" t="s">
         <v>56</v>
       </c>
-      <c r="BK1" s="124"/>
-      <c r="BL1" s="124"/>
-      <c r="BM1" s="124"/>
-      <c r="BN1" s="125"/>
-      <c r="BO1" s="123" t="s">
+      <c r="BK1" s="120"/>
+      <c r="BL1" s="120"/>
+      <c r="BM1" s="120"/>
+      <c r="BN1" s="121"/>
+      <c r="BO1" s="119" t="s">
         <v>57</v>
       </c>
-      <c r="BP1" s="124"/>
-      <c r="BQ1" s="124"/>
-      <c r="BR1" s="124"/>
-      <c r="BS1" s="125"/>
-      <c r="BT1" s="123" t="s">
+      <c r="BP1" s="120"/>
+      <c r="BQ1" s="120"/>
+      <c r="BR1" s="120"/>
+      <c r="BS1" s="121"/>
+      <c r="BT1" s="119" t="s">
         <v>58</v>
       </c>
-      <c r="BU1" s="124"/>
-      <c r="BV1" s="124"/>
-      <c r="BW1" s="124"/>
-      <c r="BX1" s="125"/>
-      <c r="BY1" s="123" t="s">
+      <c r="BU1" s="120"/>
+      <c r="BV1" s="120"/>
+      <c r="BW1" s="120"/>
+      <c r="BX1" s="121"/>
+      <c r="BY1" s="119" t="s">
         <v>59</v>
       </c>
-      <c r="BZ1" s="124"/>
-      <c r="CA1" s="124"/>
-      <c r="CB1" s="124"/>
-      <c r="CC1" s="125"/>
-      <c r="CD1" s="123" t="s">
+      <c r="BZ1" s="120"/>
+      <c r="CA1" s="120"/>
+      <c r="CB1" s="120"/>
+      <c r="CC1" s="121"/>
+      <c r="CD1" s="119" t="s">
         <v>60</v>
       </c>
-      <c r="CE1" s="124"/>
-      <c r="CF1" s="124"/>
-      <c r="CG1" s="124"/>
-      <c r="CH1" s="125"/>
-      <c r="CI1" s="123" t="s">
+      <c r="CE1" s="120"/>
+      <c r="CF1" s="120"/>
+      <c r="CG1" s="120"/>
+      <c r="CH1" s="121"/>
+      <c r="CI1" s="119" t="s">
         <v>8</v>
       </c>
-      <c r="CJ1" s="124"/>
-      <c r="CK1" s="124"/>
-      <c r="CL1" s="124"/>
-      <c r="CM1" s="125"/>
-      <c r="CN1" s="123" t="s">
+      <c r="CJ1" s="120"/>
+      <c r="CK1" s="120"/>
+      <c r="CL1" s="120"/>
+      <c r="CM1" s="121"/>
+      <c r="CN1" s="119" t="s">
         <v>61</v>
       </c>
-      <c r="CO1" s="124"/>
-      <c r="CP1" s="124"/>
-      <c r="CQ1" s="124"/>
-      <c r="CR1" s="125"/>
-      <c r="CS1" s="123" t="s">
+      <c r="CO1" s="120"/>
+      <c r="CP1" s="120"/>
+      <c r="CQ1" s="120"/>
+      <c r="CR1" s="121"/>
+      <c r="CS1" s="119" t="s">
         <v>9</v>
       </c>
-      <c r="CT1" s="124"/>
-      <c r="CU1" s="124"/>
-      <c r="CV1" s="124"/>
-      <c r="CW1" s="125"/>
-      <c r="CX1" s="123" t="s">
+      <c r="CT1" s="120"/>
+      <c r="CU1" s="120"/>
+      <c r="CV1" s="120"/>
+      <c r="CW1" s="121"/>
+      <c r="CX1" s="119" t="s">
         <v>62</v>
       </c>
-      <c r="CY1" s="124"/>
-      <c r="CZ1" s="124"/>
-      <c r="DA1" s="124"/>
-      <c r="DB1" s="125"/>
-      <c r="DC1" s="123" t="s">
+      <c r="CY1" s="120"/>
+      <c r="CZ1" s="120"/>
+      <c r="DA1" s="120"/>
+      <c r="DB1" s="121"/>
+      <c r="DC1" s="119" t="s">
         <v>10</v>
       </c>
-      <c r="DD1" s="124"/>
-      <c r="DE1" s="124"/>
-      <c r="DF1" s="124"/>
-      <c r="DG1" s="125"/>
-      <c r="DH1" s="123" t="s">
+      <c r="DD1" s="120"/>
+      <c r="DE1" s="120"/>
+      <c r="DF1" s="120"/>
+      <c r="DG1" s="121"/>
+      <c r="DH1" s="119" t="s">
         <v>63</v>
       </c>
-      <c r="DI1" s="124"/>
-      <c r="DJ1" s="124"/>
-      <c r="DK1" s="124"/>
-      <c r="DL1" s="125"/>
-      <c r="DM1" s="123" t="s">
+      <c r="DI1" s="120"/>
+      <c r="DJ1" s="120"/>
+      <c r="DK1" s="120"/>
+      <c r="DL1" s="121"/>
+      <c r="DM1" s="119" t="s">
         <v>11</v>
       </c>
-      <c r="DN1" s="124"/>
-      <c r="DO1" s="124"/>
-      <c r="DP1" s="124"/>
-      <c r="DQ1" s="125"/>
-      <c r="DR1" s="123" t="s">
+      <c r="DN1" s="120"/>
+      <c r="DO1" s="120"/>
+      <c r="DP1" s="120"/>
+      <c r="DQ1" s="121"/>
+      <c r="DR1" s="119" t="s">
         <v>64</v>
       </c>
-      <c r="DS1" s="124"/>
-      <c r="DT1" s="124"/>
-      <c r="DU1" s="124"/>
-      <c r="DV1" s="125"/>
-      <c r="DW1" s="123" t="s">
+      <c r="DS1" s="120"/>
+      <c r="DT1" s="120"/>
+      <c r="DU1" s="120"/>
+      <c r="DV1" s="121"/>
+      <c r="DW1" s="119" t="s">
         <v>65</v>
       </c>
-      <c r="DX1" s="124"/>
-      <c r="DY1" s="124"/>
-      <c r="DZ1" s="124"/>
-      <c r="EA1" s="125"/>
-      <c r="EB1" s="123" t="s">
+      <c r="DX1" s="120"/>
+      <c r="DY1" s="120"/>
+      <c r="DZ1" s="120"/>
+      <c r="EA1" s="121"/>
+      <c r="EB1" s="119" t="s">
         <v>66</v>
       </c>
-      <c r="EC1" s="124"/>
-      <c r="ED1" s="124"/>
-      <c r="EE1" s="124"/>
-      <c r="EF1" s="125"/>
-      <c r="EG1" s="123" t="s">
+      <c r="EC1" s="120"/>
+      <c r="ED1" s="120"/>
+      <c r="EE1" s="120"/>
+      <c r="EF1" s="121"/>
+      <c r="EG1" s="119" t="s">
         <v>67</v>
       </c>
-      <c r="EH1" s="124"/>
-      <c r="EI1" s="124"/>
-      <c r="EJ1" s="124"/>
-      <c r="EK1" s="125"/>
-      <c r="EL1" s="123" t="s">
+      <c r="EH1" s="120"/>
+      <c r="EI1" s="120"/>
+      <c r="EJ1" s="120"/>
+      <c r="EK1" s="121"/>
+      <c r="EL1" s="119" t="s">
         <v>68</v>
       </c>
-      <c r="EM1" s="124"/>
-      <c r="EN1" s="124"/>
-      <c r="EO1" s="124"/>
-      <c r="EP1" s="125"/>
+      <c r="EM1" s="120"/>
+      <c r="EN1" s="120"/>
+      <c r="EO1" s="120"/>
+      <c r="EP1" s="121"/>
     </row>
     <row r="2" spans="1:146" ht="12.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="1"/>
-      <c r="B2" s="132" t="s">
+      <c r="B2" s="122" t="s">
         <v>112</v>
       </c>
       <c r="C2" s="116" t="s">
@@ -1973,206 +2097,206 @@
       <c r="F2" s="116" t="s">
         <v>115</v>
       </c>
-      <c r="G2" s="129" t="s">
+      <c r="G2" s="125" t="s">
         <v>12</v>
       </c>
-      <c r="H2" s="130"/>
-      <c r="I2" s="130"/>
-      <c r="J2" s="130"/>
-      <c r="K2" s="131"/>
-      <c r="L2" s="126" t="s">
+      <c r="H2" s="126"/>
+      <c r="I2" s="126"/>
+      <c r="J2" s="126"/>
+      <c r="K2" s="127"/>
+      <c r="L2" s="128" t="s">
         <v>12</v>
       </c>
-      <c r="M2" s="127"/>
-      <c r="N2" s="127"/>
-      <c r="O2" s="127"/>
-      <c r="P2" s="128"/>
-      <c r="Q2" s="129" t="s">
+      <c r="M2" s="129"/>
+      <c r="N2" s="129"/>
+      <c r="O2" s="129"/>
+      <c r="P2" s="130"/>
+      <c r="Q2" s="125" t="s">
         <v>12</v>
       </c>
-      <c r="R2" s="130"/>
-      <c r="S2" s="130"/>
-      <c r="T2" s="130"/>
-      <c r="U2" s="131"/>
-      <c r="V2" s="126" t="s">
+      <c r="R2" s="126"/>
+      <c r="S2" s="126"/>
+      <c r="T2" s="126"/>
+      <c r="U2" s="127"/>
+      <c r="V2" s="128" t="s">
         <v>12</v>
       </c>
-      <c r="W2" s="127"/>
-      <c r="X2" s="127"/>
-      <c r="Y2" s="127"/>
-      <c r="Z2" s="128"/>
-      <c r="AA2" s="129" t="s">
+      <c r="W2" s="129"/>
+      <c r="X2" s="129"/>
+      <c r="Y2" s="129"/>
+      <c r="Z2" s="130"/>
+      <c r="AA2" s="125" t="s">
         <v>12</v>
       </c>
-      <c r="AB2" s="130"/>
-      <c r="AC2" s="130"/>
-      <c r="AD2" s="130"/>
-      <c r="AE2" s="131"/>
-      <c r="AF2" s="126" t="s">
+      <c r="AB2" s="126"/>
+      <c r="AC2" s="126"/>
+      <c r="AD2" s="126"/>
+      <c r="AE2" s="127"/>
+      <c r="AF2" s="128" t="s">
         <v>12</v>
       </c>
-      <c r="AG2" s="127"/>
-      <c r="AH2" s="127"/>
-      <c r="AI2" s="127"/>
-      <c r="AJ2" s="128"/>
-      <c r="AK2" s="129" t="s">
+      <c r="AG2" s="129"/>
+      <c r="AH2" s="129"/>
+      <c r="AI2" s="129"/>
+      <c r="AJ2" s="130"/>
+      <c r="AK2" s="125" t="s">
         <v>12</v>
       </c>
-      <c r="AL2" s="130"/>
-      <c r="AM2" s="130"/>
-      <c r="AN2" s="130"/>
-      <c r="AO2" s="131"/>
-      <c r="AP2" s="126" t="s">
+      <c r="AL2" s="126"/>
+      <c r="AM2" s="126"/>
+      <c r="AN2" s="126"/>
+      <c r="AO2" s="127"/>
+      <c r="AP2" s="128" t="s">
         <v>12</v>
       </c>
-      <c r="AQ2" s="127"/>
-      <c r="AR2" s="127"/>
-      <c r="AS2" s="127"/>
-      <c r="AT2" s="128"/>
-      <c r="AU2" s="129" t="s">
+      <c r="AQ2" s="129"/>
+      <c r="AR2" s="129"/>
+      <c r="AS2" s="129"/>
+      <c r="AT2" s="130"/>
+      <c r="AU2" s="125" t="s">
         <v>12</v>
       </c>
-      <c r="AV2" s="130"/>
-      <c r="AW2" s="130"/>
-      <c r="AX2" s="130"/>
-      <c r="AY2" s="131"/>
-      <c r="AZ2" s="126" t="s">
+      <c r="AV2" s="126"/>
+      <c r="AW2" s="126"/>
+      <c r="AX2" s="126"/>
+      <c r="AY2" s="127"/>
+      <c r="AZ2" s="128" t="s">
         <v>12</v>
       </c>
-      <c r="BA2" s="127"/>
-      <c r="BB2" s="127"/>
-      <c r="BC2" s="127"/>
-      <c r="BD2" s="128"/>
-      <c r="BE2" s="129" t="s">
+      <c r="BA2" s="129"/>
+      <c r="BB2" s="129"/>
+      <c r="BC2" s="129"/>
+      <c r="BD2" s="130"/>
+      <c r="BE2" s="125" t="s">
         <v>12</v>
       </c>
-      <c r="BF2" s="130"/>
-      <c r="BG2" s="130"/>
-      <c r="BH2" s="130"/>
-      <c r="BI2" s="131"/>
-      <c r="BJ2" s="126" t="s">
+      <c r="BF2" s="126"/>
+      <c r="BG2" s="126"/>
+      <c r="BH2" s="126"/>
+      <c r="BI2" s="127"/>
+      <c r="BJ2" s="128" t="s">
         <v>12</v>
       </c>
-      <c r="BK2" s="127"/>
-      <c r="BL2" s="127"/>
-      <c r="BM2" s="127"/>
-      <c r="BN2" s="128"/>
-      <c r="BO2" s="129" t="s">
+      <c r="BK2" s="129"/>
+      <c r="BL2" s="129"/>
+      <c r="BM2" s="129"/>
+      <c r="BN2" s="130"/>
+      <c r="BO2" s="125" t="s">
         <v>12</v>
       </c>
-      <c r="BP2" s="130"/>
-      <c r="BQ2" s="130"/>
-      <c r="BR2" s="130"/>
-      <c r="BS2" s="131"/>
-      <c r="BT2" s="126" t="s">
+      <c r="BP2" s="126"/>
+      <c r="BQ2" s="126"/>
+      <c r="BR2" s="126"/>
+      <c r="BS2" s="127"/>
+      <c r="BT2" s="128" t="s">
         <v>12</v>
       </c>
-      <c r="BU2" s="127"/>
-      <c r="BV2" s="127"/>
-      <c r="BW2" s="127"/>
-      <c r="BX2" s="128"/>
-      <c r="BY2" s="129" t="s">
+      <c r="BU2" s="129"/>
+      <c r="BV2" s="129"/>
+      <c r="BW2" s="129"/>
+      <c r="BX2" s="130"/>
+      <c r="BY2" s="125" t="s">
         <v>12</v>
       </c>
-      <c r="BZ2" s="130"/>
-      <c r="CA2" s="130"/>
-      <c r="CB2" s="130"/>
-      <c r="CC2" s="131"/>
-      <c r="CD2" s="126" t="s">
+      <c r="BZ2" s="126"/>
+      <c r="CA2" s="126"/>
+      <c r="CB2" s="126"/>
+      <c r="CC2" s="127"/>
+      <c r="CD2" s="128" t="s">
         <v>12</v>
       </c>
-      <c r="CE2" s="127"/>
-      <c r="CF2" s="127"/>
-      <c r="CG2" s="127"/>
-      <c r="CH2" s="128"/>
-      <c r="CI2" s="129" t="s">
+      <c r="CE2" s="129"/>
+      <c r="CF2" s="129"/>
+      <c r="CG2" s="129"/>
+      <c r="CH2" s="130"/>
+      <c r="CI2" s="125" t="s">
         <v>12</v>
       </c>
-      <c r="CJ2" s="130"/>
-      <c r="CK2" s="130"/>
-      <c r="CL2" s="130"/>
-      <c r="CM2" s="131"/>
-      <c r="CN2" s="126" t="s">
+      <c r="CJ2" s="126"/>
+      <c r="CK2" s="126"/>
+      <c r="CL2" s="126"/>
+      <c r="CM2" s="127"/>
+      <c r="CN2" s="128" t="s">
         <v>12</v>
       </c>
-      <c r="CO2" s="127"/>
-      <c r="CP2" s="127"/>
-      <c r="CQ2" s="127"/>
-      <c r="CR2" s="128"/>
-      <c r="CS2" s="129" t="s">
+      <c r="CO2" s="129"/>
+      <c r="CP2" s="129"/>
+      <c r="CQ2" s="129"/>
+      <c r="CR2" s="130"/>
+      <c r="CS2" s="125" t="s">
         <v>12</v>
       </c>
-      <c r="CT2" s="130"/>
-      <c r="CU2" s="130"/>
-      <c r="CV2" s="130"/>
-      <c r="CW2" s="131"/>
-      <c r="CX2" s="126" t="s">
+      <c r="CT2" s="126"/>
+      <c r="CU2" s="126"/>
+      <c r="CV2" s="126"/>
+      <c r="CW2" s="127"/>
+      <c r="CX2" s="128" t="s">
         <v>12</v>
       </c>
-      <c r="CY2" s="127"/>
-      <c r="CZ2" s="127"/>
-      <c r="DA2" s="127"/>
-      <c r="DB2" s="128"/>
-      <c r="DC2" s="129" t="s">
+      <c r="CY2" s="129"/>
+      <c r="CZ2" s="129"/>
+      <c r="DA2" s="129"/>
+      <c r="DB2" s="130"/>
+      <c r="DC2" s="125" t="s">
         <v>12</v>
       </c>
-      <c r="DD2" s="130"/>
-      <c r="DE2" s="130"/>
-      <c r="DF2" s="130"/>
-      <c r="DG2" s="131"/>
-      <c r="DH2" s="126" t="s">
+      <c r="DD2" s="126"/>
+      <c r="DE2" s="126"/>
+      <c r="DF2" s="126"/>
+      <c r="DG2" s="127"/>
+      <c r="DH2" s="128" t="s">
         <v>12</v>
       </c>
-      <c r="DI2" s="127"/>
-      <c r="DJ2" s="127"/>
-      <c r="DK2" s="127"/>
-      <c r="DL2" s="128"/>
-      <c r="DM2" s="129" t="s">
+      <c r="DI2" s="129"/>
+      <c r="DJ2" s="129"/>
+      <c r="DK2" s="129"/>
+      <c r="DL2" s="130"/>
+      <c r="DM2" s="125" t="s">
         <v>12</v>
       </c>
-      <c r="DN2" s="130"/>
-      <c r="DO2" s="130"/>
-      <c r="DP2" s="130"/>
-      <c r="DQ2" s="131"/>
-      <c r="DR2" s="126" t="s">
+      <c r="DN2" s="126"/>
+      <c r="DO2" s="126"/>
+      <c r="DP2" s="126"/>
+      <c r="DQ2" s="127"/>
+      <c r="DR2" s="128" t="s">
         <v>12</v>
       </c>
-      <c r="DS2" s="127"/>
-      <c r="DT2" s="127"/>
-      <c r="DU2" s="127"/>
-      <c r="DV2" s="128"/>
-      <c r="DW2" s="129" t="s">
+      <c r="DS2" s="129"/>
+      <c r="DT2" s="129"/>
+      <c r="DU2" s="129"/>
+      <c r="DV2" s="130"/>
+      <c r="DW2" s="125" t="s">
         <v>12</v>
       </c>
-      <c r="DX2" s="130"/>
-      <c r="DY2" s="130"/>
-      <c r="DZ2" s="130"/>
-      <c r="EA2" s="131"/>
-      <c r="EB2" s="126" t="s">
+      <c r="DX2" s="126"/>
+      <c r="DY2" s="126"/>
+      <c r="DZ2" s="126"/>
+      <c r="EA2" s="127"/>
+      <c r="EB2" s="128" t="s">
         <v>12</v>
       </c>
-      <c r="EC2" s="127"/>
-      <c r="ED2" s="127"/>
-      <c r="EE2" s="127"/>
-      <c r="EF2" s="128"/>
-      <c r="EG2" s="129" t="s">
+      <c r="EC2" s="129"/>
+      <c r="ED2" s="129"/>
+      <c r="EE2" s="129"/>
+      <c r="EF2" s="130"/>
+      <c r="EG2" s="125" t="s">
         <v>12</v>
       </c>
-      <c r="EH2" s="130"/>
-      <c r="EI2" s="130"/>
-      <c r="EJ2" s="130"/>
-      <c r="EK2" s="131"/>
-      <c r="EL2" s="126" t="s">
+      <c r="EH2" s="126"/>
+      <c r="EI2" s="126"/>
+      <c r="EJ2" s="126"/>
+      <c r="EK2" s="127"/>
+      <c r="EL2" s="128" t="s">
         <v>12</v>
       </c>
-      <c r="EM2" s="127"/>
-      <c r="EN2" s="127"/>
-      <c r="EO2" s="127"/>
-      <c r="EP2" s="128"/>
+      <c r="EM2" s="129"/>
+      <c r="EN2" s="129"/>
+      <c r="EO2" s="129"/>
+      <c r="EP2" s="130"/>
     </row>
     <row r="3" spans="1:146" x14ac:dyDescent="0.2">
       <c r="A3" s="69"/>
-      <c r="B3" s="133"/>
+      <c r="B3" s="123"/>
       <c r="C3" s="117"/>
       <c r="D3" s="117"/>
       <c r="E3" s="117"/>
@@ -2600,7 +2724,7 @@
     </row>
     <row r="4" spans="1:146" x14ac:dyDescent="0.2">
       <c r="A4" s="69"/>
-      <c r="B4" s="133"/>
+      <c r="B4" s="123"/>
       <c r="C4" s="117"/>
       <c r="D4" s="117"/>
       <c r="E4" s="117"/>
@@ -3028,7 +3152,7 @@
     </row>
     <row r="5" spans="1:146" x14ac:dyDescent="0.2">
       <c r="A5" s="69"/>
-      <c r="B5" s="134"/>
+      <c r="B5" s="124"/>
       <c r="C5" s="118"/>
       <c r="D5" s="118"/>
       <c r="E5" s="118"/>
@@ -3990,10 +4114,10 @@
         <v>91368</v>
       </c>
       <c r="AG7" s="30">
-        <v>81918.600000000006</v>
+        <v>0</v>
       </c>
       <c r="AH7" s="30">
-        <v>87466.1</v>
+        <v>0</v>
       </c>
       <c r="AI7" s="30">
         <v>84220</v>
@@ -4430,10 +4554,10 @@
         <v>0</v>
       </c>
       <c r="AG8" s="24">
-        <v>23107.1</v>
+        <v>0</v>
       </c>
       <c r="AH8" s="24">
-        <v>23319.3</v>
+        <v>0</v>
       </c>
       <c r="AI8" s="24">
         <v>21280</v>
@@ -4870,10 +4994,10 @@
         <v>0</v>
       </c>
       <c r="AG9" s="24">
-        <v>29179.600000000002</v>
+        <v>0</v>
       </c>
       <c r="AH9" s="24">
-        <v>34377.699999999997</v>
+        <v>0</v>
       </c>
       <c r="AI9" s="24">
         <v>31080</v>
@@ -5310,10 +5434,10 @@
         <v>0</v>
       </c>
       <c r="AG10" s="24">
-        <v>2905.9</v>
+        <v>0</v>
       </c>
       <c r="AH10" s="24">
-        <v>2874.2999999999997</v>
+        <v>0</v>
       </c>
       <c r="AI10" s="24">
         <v>3840</v>
@@ -5750,10 +5874,10 @@
         <v>0</v>
       </c>
       <c r="AG11" s="24">
-        <v>26726</v>
+        <v>0</v>
       </c>
       <c r="AH11" s="24">
-        <v>26894.799999999999</v>
+        <v>0</v>
       </c>
       <c r="AI11" s="24">
         <v>28020</v>
@@ -7510,10 +7634,10 @@
         <v>0</v>
       </c>
       <c r="AG15" s="24">
-        <v>26726</v>
+        <v>0</v>
       </c>
       <c r="AH15" s="24">
-        <v>26894.799999999999</v>
+        <v>0</v>
       </c>
       <c r="AI15" s="24">
         <v>28020</v>
@@ -9710,10 +9834,10 @@
         <v>12068</v>
       </c>
       <c r="AG20" s="43">
-        <v>12696</v>
+        <v>0</v>
       </c>
       <c r="AH20" s="43">
-        <v>12696</v>
+        <v>0</v>
       </c>
       <c r="AI20" s="43">
         <v>12050</v>
@@ -10150,10 +10274,10 @@
         <v>82261</v>
       </c>
       <c r="AG21" s="48">
-        <v>87463</v>
+        <v>0</v>
       </c>
       <c r="AH21" s="48">
-        <v>94639.5</v>
+        <v>0</v>
       </c>
       <c r="AI21" s="48">
         <v>81450</v>
@@ -10590,10 +10714,10 @@
         <v>11240</v>
       </c>
       <c r="AG22" s="24">
-        <v>10314</v>
+        <v>0</v>
       </c>
       <c r="AH22" s="24">
-        <v>10319.5</v>
+        <v>0</v>
       </c>
       <c r="AI22" s="24">
         <v>11150</v>
@@ -13230,10 +13354,10 @@
         <v>11240</v>
       </c>
       <c r="AG28" s="24">
-        <v>10314</v>
+        <v>0</v>
       </c>
       <c r="AH28" s="24">
-        <v>10319.5</v>
+        <v>0</v>
       </c>
       <c r="AI28" s="24">
         <v>11150</v>
@@ -13670,10 +13794,10 @@
         <v>34660</v>
       </c>
       <c r="AG29" s="24">
-        <v>34271</v>
+        <v>0</v>
       </c>
       <c r="AH29" s="24">
-        <v>39193</v>
+        <v>0</v>
       </c>
       <c r="AI29" s="24">
         <v>31600</v>
@@ -14990,10 +15114,10 @@
         <v>34660</v>
       </c>
       <c r="AG32" s="24">
-        <v>34271</v>
+        <v>0</v>
       </c>
       <c r="AH32" s="24">
-        <v>39193</v>
+        <v>0</v>
       </c>
       <c r="AI32" s="24">
         <v>0</v>
@@ -15430,10 +15554,10 @@
         <v>36337</v>
       </c>
       <c r="AG33" s="24">
-        <v>36337</v>
+        <v>0</v>
       </c>
       <c r="AH33" s="24">
-        <v>38236</v>
+        <v>0</v>
       </c>
       <c r="AI33" s="24">
         <v>33000</v>
@@ -16750,10 +16874,10 @@
         <v>0</v>
       </c>
       <c r="AG36" s="24">
-        <v>36337</v>
+        <v>0</v>
       </c>
       <c r="AH36" s="24">
-        <v>38236</v>
+        <v>0</v>
       </c>
       <c r="AI36" s="24">
         <v>33000</v>
@@ -17190,10 +17314,10 @@
         <v>24</v>
       </c>
       <c r="AG37" s="24">
-        <v>24</v>
+        <v>0</v>
       </c>
       <c r="AH37" s="24">
-        <v>24</v>
+        <v>0</v>
       </c>
       <c r="AI37" s="24">
         <v>0</v>
@@ -18070,10 +18194,10 @@
         <v>0</v>
       </c>
       <c r="AG39" s="24">
-        <v>6517</v>
+        <v>0</v>
       </c>
       <c r="AH39" s="24">
-        <v>6867</v>
+        <v>0</v>
       </c>
       <c r="AI39" s="24">
         <v>5700</v>
@@ -18510,10 +18634,10 @@
         <v>0</v>
       </c>
       <c r="AG40" s="24">
-        <v>6517</v>
+        <v>0</v>
       </c>
       <c r="AH40" s="24">
-        <v>6867</v>
+        <v>0</v>
       </c>
       <c r="AI40" s="24">
         <v>5700</v>
@@ -19830,10 +19954,10 @@
         <v>420</v>
       </c>
       <c r="AG43" s="59">
-        <v>7610.2999999999993</v>
+        <v>0</v>
       </c>
       <c r="AH43" s="59">
-        <v>7039</v>
+        <v>0</v>
       </c>
       <c r="AI43" s="59">
         <v>4440</v>
@@ -20270,10 +20394,10 @@
         <v>186117</v>
       </c>
       <c r="AG44" s="67">
-        <v>189687.90000000002</v>
+        <v>0</v>
       </c>
       <c r="AH44" s="67">
-        <v>201840.6</v>
+        <v>0</v>
       </c>
       <c r="AI44" s="67">
         <v>182160</v>
@@ -20634,12 +20758,12 @@
       <c r="S48" s="75"/>
       <c r="T48" s="75"/>
       <c r="U48" s="75"/>
-      <c r="V48" s="122"/>
-      <c r="W48" s="122"/>
-      <c r="X48" s="122"/>
-      <c r="Y48" s="122"/>
-      <c r="Z48" s="122"/>
-      <c r="AA48" s="122"/>
+      <c r="V48" s="134"/>
+      <c r="W48" s="134"/>
+      <c r="X48" s="134"/>
+      <c r="Y48" s="134"/>
+      <c r="Z48" s="134"/>
+      <c r="AA48" s="134"/>
     </row>
     <row r="49" spans="1:120" x14ac:dyDescent="0.2">
       <c r="A49" s="82"/>
@@ -20712,6 +20836,53 @@
   </sheetData>
   <autoFilter ref="B6:E44"/>
   <mergeCells count="63">
+    <mergeCell ref="F2:F5"/>
+    <mergeCell ref="B1:F1"/>
+    <mergeCell ref="V48:AA48"/>
+    <mergeCell ref="BJ1:BN1"/>
+    <mergeCell ref="G1:K1"/>
+    <mergeCell ref="L1:P1"/>
+    <mergeCell ref="Q1:U1"/>
+    <mergeCell ref="V1:Z1"/>
+    <mergeCell ref="AA1:AE1"/>
+    <mergeCell ref="AF1:AJ1"/>
+    <mergeCell ref="AK1:AO1"/>
+    <mergeCell ref="AP1:AT1"/>
+    <mergeCell ref="AU1:AY1"/>
+    <mergeCell ref="AZ1:BD1"/>
+    <mergeCell ref="BE1:BI1"/>
+    <mergeCell ref="BJ2:BN2"/>
+    <mergeCell ref="G2:K2"/>
+    <mergeCell ref="L2:P2"/>
+    <mergeCell ref="Q2:U2"/>
+    <mergeCell ref="V2:Z2"/>
+    <mergeCell ref="AA2:AE2"/>
+    <mergeCell ref="AF2:AJ2"/>
+    <mergeCell ref="AK2:AO2"/>
+    <mergeCell ref="BY1:CC1"/>
+    <mergeCell ref="CD1:CH1"/>
+    <mergeCell ref="CI1:CM1"/>
+    <mergeCell ref="AP2:AT2"/>
+    <mergeCell ref="AU2:AY2"/>
+    <mergeCell ref="AZ2:BD2"/>
+    <mergeCell ref="BE2:BI2"/>
+    <mergeCell ref="BO1:BS1"/>
+    <mergeCell ref="EL2:EP2"/>
+    <mergeCell ref="EL1:EP1"/>
+    <mergeCell ref="BO2:BS2"/>
+    <mergeCell ref="BT2:BX2"/>
+    <mergeCell ref="BY2:CC2"/>
+    <mergeCell ref="CD2:CH2"/>
+    <mergeCell ref="CI2:CM2"/>
+    <mergeCell ref="CN2:CR2"/>
+    <mergeCell ref="CS2:CW2"/>
+    <mergeCell ref="CX2:DB2"/>
+    <mergeCell ref="DC2:DG2"/>
+    <mergeCell ref="DH2:DL2"/>
+    <mergeCell ref="DM2:DQ2"/>
+    <mergeCell ref="CS1:CW1"/>
+    <mergeCell ref="CX1:DB1"/>
+    <mergeCell ref="DC1:DG1"/>
     <mergeCell ref="C2:C5"/>
     <mergeCell ref="D2:D5"/>
     <mergeCell ref="E2:E5"/>
@@ -20728,53 +20899,6 @@
     <mergeCell ref="DW2:EA2"/>
     <mergeCell ref="BT1:BX1"/>
     <mergeCell ref="CN1:CR1"/>
-    <mergeCell ref="EL2:EP2"/>
-    <mergeCell ref="EL1:EP1"/>
-    <mergeCell ref="BO2:BS2"/>
-    <mergeCell ref="BT2:BX2"/>
-    <mergeCell ref="BY2:CC2"/>
-    <mergeCell ref="CD2:CH2"/>
-    <mergeCell ref="CI2:CM2"/>
-    <mergeCell ref="CN2:CR2"/>
-    <mergeCell ref="CS2:CW2"/>
-    <mergeCell ref="CX2:DB2"/>
-    <mergeCell ref="DC2:DG2"/>
-    <mergeCell ref="DH2:DL2"/>
-    <mergeCell ref="DM2:DQ2"/>
-    <mergeCell ref="CS1:CW1"/>
-    <mergeCell ref="CX1:DB1"/>
-    <mergeCell ref="DC1:DG1"/>
-    <mergeCell ref="AF2:AJ2"/>
-    <mergeCell ref="AK2:AO2"/>
-    <mergeCell ref="BY1:CC1"/>
-    <mergeCell ref="CD1:CH1"/>
-    <mergeCell ref="CI1:CM1"/>
-    <mergeCell ref="AP2:AT2"/>
-    <mergeCell ref="AU2:AY2"/>
-    <mergeCell ref="AZ2:BD2"/>
-    <mergeCell ref="BE2:BI2"/>
-    <mergeCell ref="BO1:BS1"/>
-    <mergeCell ref="G2:K2"/>
-    <mergeCell ref="L2:P2"/>
-    <mergeCell ref="Q2:U2"/>
-    <mergeCell ref="V2:Z2"/>
-    <mergeCell ref="AA2:AE2"/>
-    <mergeCell ref="F2:F5"/>
-    <mergeCell ref="B1:F1"/>
-    <mergeCell ref="V48:AA48"/>
-    <mergeCell ref="BJ1:BN1"/>
-    <mergeCell ref="G1:K1"/>
-    <mergeCell ref="L1:P1"/>
-    <mergeCell ref="Q1:U1"/>
-    <mergeCell ref="V1:Z1"/>
-    <mergeCell ref="AA1:AE1"/>
-    <mergeCell ref="AF1:AJ1"/>
-    <mergeCell ref="AK1:AO1"/>
-    <mergeCell ref="AP1:AT1"/>
-    <mergeCell ref="AU1:AY1"/>
-    <mergeCell ref="AZ1:BD1"/>
-    <mergeCell ref="BE1:BI1"/>
-    <mergeCell ref="BJ2:BN2"/>
   </mergeCells>
   <conditionalFormatting sqref="B7:F44">
     <cfRule type="cellIs" dxfId="0" priority="1" operator="equal">

</xml_diff>

<commit_message>
- Minor adjustments in the script
</commit_message>
<xml_diff>
--- a/input/National_Generation_Capacities.xlsx
+++ b/input/National_Generation_Capacities.xlsx
@@ -9,10 +9,11 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="480" yWindow="240" windowWidth="24540" windowHeight="11955"/>
+    <workbookView xWindow="480" yWindow="240" windowWidth="24540" windowHeight="11955" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="Summary" sheetId="1" r:id="rId1"/>
+    <sheet name="Additional notes" sheetId="2" r:id="rId2"/>
   </sheets>
   <definedNames>
     <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Summary!$B$6:$E$45</definedName>
@@ -22,7 +23,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3696" uniqueCount="123">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="3705" uniqueCount="132">
   <si>
     <t>AT</t>
   </si>
@@ -392,6 +393,33 @@
   <si>
     <t>Department of Energy &amp; Climate Change</t>
   </si>
+  <si>
+    <t>Additional notes</t>
+  </si>
+  <si>
+    <t>"Differently categorized …"</t>
+  </si>
+  <si>
+    <t>"Reservoir including pumped storage"</t>
+  </si>
+  <si>
+    <t>"Pumped storage with natural inflow"</t>
+  </si>
+  <si>
+    <t>Pumped storage with natural inflow, or reservoirs with pumping capacity.</t>
+  </si>
+  <si>
+    <t>Aggregated capacity of reservoirs and pumped storage, or combinations of both. Relevant for AT.</t>
+  </si>
+  <si>
+    <t>The relation between individual categories and energy source levels is laid down in the additional sheet 'technology levels'.</t>
+  </si>
+  <si>
+    <t xml:space="preserve">These categories comprise either capacities which cannot be assigned to specific categories at the same level, or capacities with unspecified fuel or technology. </t>
+  </si>
+  <si>
+    <t>The categories used in the dataset cover different levels, so called energy source levels, to reflect the structural relations among the categories. Moreover, this ensures that the total capacity is identical for each energy source level.</t>
+  </si>
 </sst>
 </file>
 
@@ -402,7 +430,7 @@
     <numFmt numFmtId="164" formatCode="0_ ;\-0\ "/>
     <numFmt numFmtId="165" formatCode="#,##0.00_ ;\-#,##0.00\ "/>
   </numFmts>
-  <fonts count="8" x14ac:knownFonts="1">
+  <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color theme="1"/>
@@ -455,6 +483,20 @@
       <sz val="11"/>
       <color theme="1"/>
       <name val="Calibri"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <i/>
+      <sz val="10"/>
+      <color theme="1"/>
+      <name val="Arial"/>
       <family val="2"/>
     </font>
   </fonts>
@@ -950,7 +992,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="139">
+  <cellXfs count="141">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="49" fontId="3" fillId="3" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1296,15 +1338,8 @@
     <xf numFmtId="165" fontId="6" fillId="8" borderId="20" xfId="1" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
+    <xf numFmtId="0" fontId="8" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="5" fillId="7" borderId="28" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
@@ -1321,6 +1356,15 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="7" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="4" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="5" fillId="7" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -2052,8 +2096,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:FI54"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
-      <selection activeCell="E43" sqref="E43"/>
+    <sheetView zoomScale="70" zoomScaleNormal="70" workbookViewId="0">
+      <selection activeCell="H25" sqref="H25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -2067,469 +2111,469 @@
   <sheetData>
     <row r="1" spans="1:165" s="16" customFormat="1" ht="15.75" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A1" s="14"/>
-      <c r="B1" s="127" t="s">
+      <c r="B1" s="126" t="s">
         <v>115</v>
       </c>
-      <c r="C1" s="128"/>
-      <c r="D1" s="128"/>
-      <c r="E1" s="128"/>
-      <c r="F1" s="129"/>
-      <c r="G1" s="121" t="s">
-        <v>0</v>
-      </c>
-      <c r="H1" s="122"/>
-      <c r="I1" s="122"/>
-      <c r="J1" s="122"/>
-      <c r="K1" s="122"/>
-      <c r="L1" s="123"/>
-      <c r="M1" s="121" t="s">
+      <c r="C1" s="127"/>
+      <c r="D1" s="127"/>
+      <c r="E1" s="127"/>
+      <c r="F1" s="128"/>
+      <c r="G1" s="129" t="s">
+        <v>0</v>
+      </c>
+      <c r="H1" s="130"/>
+      <c r="I1" s="130"/>
+      <c r="J1" s="130"/>
+      <c r="K1" s="130"/>
+      <c r="L1" s="131"/>
+      <c r="M1" s="129" t="s">
         <v>1</v>
       </c>
-      <c r="N1" s="122"/>
-      <c r="O1" s="122"/>
-      <c r="P1" s="122"/>
-      <c r="Q1" s="122"/>
-      <c r="R1" s="123"/>
-      <c r="S1" s="121" t="s">
+      <c r="N1" s="130"/>
+      <c r="O1" s="130"/>
+      <c r="P1" s="130"/>
+      <c r="Q1" s="130"/>
+      <c r="R1" s="131"/>
+      <c r="S1" s="129" t="s">
         <v>53</v>
       </c>
-      <c r="T1" s="122"/>
-      <c r="U1" s="122"/>
-      <c r="V1" s="122"/>
-      <c r="W1" s="123"/>
-      <c r="X1" s="121" t="s">
+      <c r="T1" s="130"/>
+      <c r="U1" s="130"/>
+      <c r="V1" s="130"/>
+      <c r="W1" s="131"/>
+      <c r="X1" s="129" t="s">
         <v>2</v>
       </c>
-      <c r="Y1" s="122"/>
-      <c r="Z1" s="122"/>
-      <c r="AA1" s="122"/>
-      <c r="AB1" s="122"/>
-      <c r="AC1" s="123"/>
-      <c r="AD1" s="121" t="s">
+      <c r="Y1" s="130"/>
+      <c r="Z1" s="130"/>
+      <c r="AA1" s="130"/>
+      <c r="AB1" s="130"/>
+      <c r="AC1" s="131"/>
+      <c r="AD1" s="129" t="s">
         <v>3</v>
       </c>
-      <c r="AE1" s="122"/>
-      <c r="AF1" s="122"/>
-      <c r="AG1" s="122"/>
-      <c r="AH1" s="122"/>
-      <c r="AI1" s="123"/>
-      <c r="AJ1" s="121" t="s">
+      <c r="AE1" s="130"/>
+      <c r="AF1" s="130"/>
+      <c r="AG1" s="130"/>
+      <c r="AH1" s="130"/>
+      <c r="AI1" s="131"/>
+      <c r="AJ1" s="129" t="s">
         <v>4</v>
       </c>
-      <c r="AK1" s="122"/>
-      <c r="AL1" s="122"/>
-      <c r="AM1" s="122"/>
-      <c r="AN1" s="123"/>
-      <c r="AO1" s="121" t="s">
+      <c r="AK1" s="130"/>
+      <c r="AL1" s="130"/>
+      <c r="AM1" s="130"/>
+      <c r="AN1" s="131"/>
+      <c r="AO1" s="129" t="s">
         <v>5</v>
       </c>
-      <c r="AP1" s="122"/>
-      <c r="AQ1" s="122"/>
-      <c r="AR1" s="122"/>
-      <c r="AS1" s="123"/>
-      <c r="AT1" s="121" t="s">
+      <c r="AP1" s="130"/>
+      <c r="AQ1" s="130"/>
+      <c r="AR1" s="130"/>
+      <c r="AS1" s="131"/>
+      <c r="AT1" s="129" t="s">
         <v>54</v>
       </c>
-      <c r="AU1" s="122"/>
-      <c r="AV1" s="122"/>
-      <c r="AW1" s="122"/>
-      <c r="AX1" s="122"/>
-      <c r="AY1" s="123"/>
-      <c r="AZ1" s="121" t="s">
+      <c r="AU1" s="130"/>
+      <c r="AV1" s="130"/>
+      <c r="AW1" s="130"/>
+      <c r="AX1" s="130"/>
+      <c r="AY1" s="131"/>
+      <c r="AZ1" s="129" t="s">
         <v>6</v>
       </c>
-      <c r="BA1" s="122"/>
-      <c r="BB1" s="122"/>
-      <c r="BC1" s="122"/>
-      <c r="BD1" s="122"/>
-      <c r="BE1" s="123"/>
-      <c r="BF1" s="121" t="s">
+      <c r="BA1" s="130"/>
+      <c r="BB1" s="130"/>
+      <c r="BC1" s="130"/>
+      <c r="BD1" s="130"/>
+      <c r="BE1" s="131"/>
+      <c r="BF1" s="129" t="s">
         <v>7</v>
       </c>
-      <c r="BG1" s="122"/>
-      <c r="BH1" s="122"/>
-      <c r="BI1" s="122"/>
-      <c r="BJ1" s="122"/>
-      <c r="BK1" s="122"/>
-      <c r="BL1" s="123"/>
-      <c r="BM1" s="121" t="s">
+      <c r="BG1" s="130"/>
+      <c r="BH1" s="130"/>
+      <c r="BI1" s="130"/>
+      <c r="BJ1" s="130"/>
+      <c r="BK1" s="130"/>
+      <c r="BL1" s="131"/>
+      <c r="BM1" s="129" t="s">
         <v>55</v>
       </c>
-      <c r="BN1" s="122"/>
-      <c r="BO1" s="122"/>
-      <c r="BP1" s="122"/>
-      <c r="BQ1" s="122"/>
-      <c r="BR1" s="123"/>
-      <c r="BS1" s="121" t="s">
+      <c r="BN1" s="130"/>
+      <c r="BO1" s="130"/>
+      <c r="BP1" s="130"/>
+      <c r="BQ1" s="130"/>
+      <c r="BR1" s="131"/>
+      <c r="BS1" s="129" t="s">
         <v>56</v>
       </c>
-      <c r="BT1" s="122"/>
-      <c r="BU1" s="122"/>
-      <c r="BV1" s="122"/>
-      <c r="BW1" s="122"/>
-      <c r="BX1" s="123"/>
-      <c r="BY1" s="121" t="s">
+      <c r="BT1" s="130"/>
+      <c r="BU1" s="130"/>
+      <c r="BV1" s="130"/>
+      <c r="BW1" s="130"/>
+      <c r="BX1" s="131"/>
+      <c r="BY1" s="129" t="s">
         <v>57</v>
       </c>
-      <c r="BZ1" s="122"/>
-      <c r="CA1" s="122"/>
-      <c r="CB1" s="122"/>
-      <c r="CC1" s="123"/>
-      <c r="CD1" s="121" t="s">
+      <c r="BZ1" s="130"/>
+      <c r="CA1" s="130"/>
+      <c r="CB1" s="130"/>
+      <c r="CC1" s="131"/>
+      <c r="CD1" s="129" t="s">
         <v>58</v>
       </c>
-      <c r="CE1" s="122"/>
-      <c r="CF1" s="122"/>
-      <c r="CG1" s="122"/>
-      <c r="CH1" s="122"/>
-      <c r="CI1" s="123"/>
-      <c r="CJ1" s="121" t="s">
+      <c r="CE1" s="130"/>
+      <c r="CF1" s="130"/>
+      <c r="CG1" s="130"/>
+      <c r="CH1" s="130"/>
+      <c r="CI1" s="131"/>
+      <c r="CJ1" s="129" t="s">
         <v>59</v>
       </c>
-      <c r="CK1" s="122"/>
-      <c r="CL1" s="122"/>
-      <c r="CM1" s="122"/>
-      <c r="CN1" s="123"/>
-      <c r="CO1" s="121" t="s">
+      <c r="CK1" s="130"/>
+      <c r="CL1" s="130"/>
+      <c r="CM1" s="130"/>
+      <c r="CN1" s="131"/>
+      <c r="CO1" s="129" t="s">
         <v>60</v>
       </c>
-      <c r="CP1" s="122"/>
-      <c r="CQ1" s="122"/>
-      <c r="CR1" s="122"/>
-      <c r="CS1" s="123"/>
-      <c r="CT1" s="121" t="s">
+      <c r="CP1" s="130"/>
+      <c r="CQ1" s="130"/>
+      <c r="CR1" s="130"/>
+      <c r="CS1" s="131"/>
+      <c r="CT1" s="129" t="s">
         <v>8</v>
       </c>
-      <c r="CU1" s="122"/>
-      <c r="CV1" s="122"/>
-      <c r="CW1" s="122"/>
-      <c r="CX1" s="123"/>
-      <c r="CY1" s="121" t="s">
+      <c r="CU1" s="130"/>
+      <c r="CV1" s="130"/>
+      <c r="CW1" s="130"/>
+      <c r="CX1" s="131"/>
+      <c r="CY1" s="129" t="s">
         <v>61</v>
       </c>
-      <c r="CZ1" s="122"/>
-      <c r="DA1" s="122"/>
-      <c r="DB1" s="122"/>
-      <c r="DC1" s="122"/>
-      <c r="DD1" s="123"/>
-      <c r="DE1" s="121" t="s">
+      <c r="CZ1" s="130"/>
+      <c r="DA1" s="130"/>
+      <c r="DB1" s="130"/>
+      <c r="DC1" s="130"/>
+      <c r="DD1" s="131"/>
+      <c r="DE1" s="129" t="s">
         <v>9</v>
       </c>
-      <c r="DF1" s="122"/>
-      <c r="DG1" s="122"/>
-      <c r="DH1" s="122"/>
-      <c r="DI1" s="123"/>
-      <c r="DJ1" s="121" t="s">
+      <c r="DF1" s="130"/>
+      <c r="DG1" s="130"/>
+      <c r="DH1" s="130"/>
+      <c r="DI1" s="131"/>
+      <c r="DJ1" s="129" t="s">
         <v>62</v>
       </c>
-      <c r="DK1" s="122"/>
-      <c r="DL1" s="122"/>
-      <c r="DM1" s="122"/>
-      <c r="DN1" s="122"/>
-      <c r="DO1" s="123"/>
-      <c r="DP1" s="121" t="s">
+      <c r="DK1" s="130"/>
+      <c r="DL1" s="130"/>
+      <c r="DM1" s="130"/>
+      <c r="DN1" s="130"/>
+      <c r="DO1" s="131"/>
+      <c r="DP1" s="129" t="s">
         <v>10</v>
       </c>
-      <c r="DQ1" s="122"/>
-      <c r="DR1" s="122"/>
-      <c r="DS1" s="122"/>
-      <c r="DT1" s="122"/>
-      <c r="DU1" s="123"/>
-      <c r="DV1" s="121" t="s">
+      <c r="DQ1" s="130"/>
+      <c r="DR1" s="130"/>
+      <c r="DS1" s="130"/>
+      <c r="DT1" s="130"/>
+      <c r="DU1" s="131"/>
+      <c r="DV1" s="129" t="s">
         <v>63</v>
       </c>
-      <c r="DW1" s="122"/>
-      <c r="DX1" s="122"/>
-      <c r="DY1" s="122"/>
-      <c r="DZ1" s="123"/>
-      <c r="EA1" s="121" t="s">
+      <c r="DW1" s="130"/>
+      <c r="DX1" s="130"/>
+      <c r="DY1" s="130"/>
+      <c r="DZ1" s="131"/>
+      <c r="EA1" s="129" t="s">
         <v>11</v>
       </c>
-      <c r="EB1" s="122"/>
-      <c r="EC1" s="122"/>
-      <c r="ED1" s="122"/>
-      <c r="EE1" s="123"/>
-      <c r="EF1" s="121" t="s">
+      <c r="EB1" s="130"/>
+      <c r="EC1" s="130"/>
+      <c r="ED1" s="130"/>
+      <c r="EE1" s="131"/>
+      <c r="EF1" s="129" t="s">
         <v>64</v>
       </c>
-      <c r="EG1" s="122"/>
-      <c r="EH1" s="122"/>
-      <c r="EI1" s="122"/>
-      <c r="EJ1" s="122"/>
-      <c r="EK1" s="123"/>
-      <c r="EL1" s="121" t="s">
+      <c r="EG1" s="130"/>
+      <c r="EH1" s="130"/>
+      <c r="EI1" s="130"/>
+      <c r="EJ1" s="130"/>
+      <c r="EK1" s="131"/>
+      <c r="EL1" s="129" t="s">
         <v>65</v>
       </c>
-      <c r="EM1" s="122"/>
-      <c r="EN1" s="122"/>
-      <c r="EO1" s="122"/>
-      <c r="EP1" s="122"/>
-      <c r="EQ1" s="123"/>
-      <c r="ER1" s="121" t="s">
+      <c r="EM1" s="130"/>
+      <c r="EN1" s="130"/>
+      <c r="EO1" s="130"/>
+      <c r="EP1" s="130"/>
+      <c r="EQ1" s="131"/>
+      <c r="ER1" s="129" t="s">
         <v>66</v>
       </c>
-      <c r="ES1" s="122"/>
-      <c r="ET1" s="122"/>
-      <c r="EU1" s="122"/>
-      <c r="EV1" s="122"/>
-      <c r="EW1" s="123"/>
-      <c r="EX1" s="121" t="s">
+      <c r="ES1" s="130"/>
+      <c r="ET1" s="130"/>
+      <c r="EU1" s="130"/>
+      <c r="EV1" s="130"/>
+      <c r="EW1" s="131"/>
+      <c r="EX1" s="129" t="s">
         <v>67</v>
       </c>
-      <c r="EY1" s="122"/>
-      <c r="EZ1" s="122"/>
-      <c r="FA1" s="122"/>
-      <c r="FB1" s="122"/>
-      <c r="FC1" s="123"/>
-      <c r="FD1" s="121" t="s">
+      <c r="EY1" s="130"/>
+      <c r="EZ1" s="130"/>
+      <c r="FA1" s="130"/>
+      <c r="FB1" s="130"/>
+      <c r="FC1" s="131"/>
+      <c r="FD1" s="129" t="s">
         <v>68</v>
       </c>
-      <c r="FE1" s="122"/>
-      <c r="FF1" s="122"/>
-      <c r="FG1" s="122"/>
-      <c r="FH1" s="122"/>
-      <c r="FI1" s="123"/>
+      <c r="FE1" s="130"/>
+      <c r="FF1" s="130"/>
+      <c r="FG1" s="130"/>
+      <c r="FH1" s="130"/>
+      <c r="FI1" s="131"/>
     </row>
     <row r="2" spans="1:165" ht="12.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A2" s="1"/>
-      <c r="B2" s="130" t="s">
+      <c r="B2" s="132" t="s">
         <v>111</v>
       </c>
-      <c r="C2" s="124" t="s">
+      <c r="C2" s="123" t="s">
         <v>112</v>
       </c>
-      <c r="D2" s="124" t="s">
+      <c r="D2" s="123" t="s">
         <v>113</v>
       </c>
-      <c r="E2" s="124" t="s">
+      <c r="E2" s="123" t="s">
         <v>118</v>
       </c>
-      <c r="F2" s="124" t="s">
+      <c r="F2" s="123" t="s">
         <v>114</v>
       </c>
-      <c r="G2" s="133" t="s">
+      <c r="G2" s="135" t="s">
         <v>12</v>
       </c>
-      <c r="H2" s="134"/>
-      <c r="I2" s="134"/>
-      <c r="J2" s="134"/>
-      <c r="K2" s="134"/>
-      <c r="L2" s="135"/>
-      <c r="M2" s="136" t="s">
+      <c r="H2" s="136"/>
+      <c r="I2" s="136"/>
+      <c r="J2" s="136"/>
+      <c r="K2" s="136"/>
+      <c r="L2" s="137"/>
+      <c r="M2" s="138" t="s">
         <v>12</v>
       </c>
-      <c r="N2" s="137"/>
-      <c r="O2" s="137"/>
-      <c r="P2" s="137"/>
-      <c r="Q2" s="137"/>
-      <c r="R2" s="138"/>
-      <c r="S2" s="133" t="s">
+      <c r="N2" s="139"/>
+      <c r="O2" s="139"/>
+      <c r="P2" s="139"/>
+      <c r="Q2" s="139"/>
+      <c r="R2" s="140"/>
+      <c r="S2" s="135" t="s">
         <v>12</v>
       </c>
-      <c r="T2" s="134"/>
-      <c r="U2" s="134"/>
-      <c r="V2" s="134"/>
-      <c r="W2" s="135"/>
-      <c r="X2" s="136" t="s">
+      <c r="T2" s="136"/>
+      <c r="U2" s="136"/>
+      <c r="V2" s="136"/>
+      <c r="W2" s="137"/>
+      <c r="X2" s="138" t="s">
         <v>12</v>
       </c>
-      <c r="Y2" s="137"/>
-      <c r="Z2" s="137"/>
-      <c r="AA2" s="137"/>
-      <c r="AB2" s="137"/>
-      <c r="AC2" s="138"/>
-      <c r="AD2" s="133" t="s">
+      <c r="Y2" s="139"/>
+      <c r="Z2" s="139"/>
+      <c r="AA2" s="139"/>
+      <c r="AB2" s="139"/>
+      <c r="AC2" s="140"/>
+      <c r="AD2" s="135" t="s">
         <v>12</v>
       </c>
-      <c r="AE2" s="134"/>
-      <c r="AF2" s="134"/>
-      <c r="AG2" s="134"/>
-      <c r="AH2" s="134"/>
-      <c r="AI2" s="135"/>
-      <c r="AJ2" s="136" t="s">
+      <c r="AE2" s="136"/>
+      <c r="AF2" s="136"/>
+      <c r="AG2" s="136"/>
+      <c r="AH2" s="136"/>
+      <c r="AI2" s="137"/>
+      <c r="AJ2" s="138" t="s">
         <v>12</v>
       </c>
-      <c r="AK2" s="137"/>
-      <c r="AL2" s="137"/>
-      <c r="AM2" s="137"/>
-      <c r="AN2" s="138"/>
-      <c r="AO2" s="133" t="s">
+      <c r="AK2" s="139"/>
+      <c r="AL2" s="139"/>
+      <c r="AM2" s="139"/>
+      <c r="AN2" s="140"/>
+      <c r="AO2" s="135" t="s">
         <v>12</v>
       </c>
-      <c r="AP2" s="134"/>
-      <c r="AQ2" s="134"/>
-      <c r="AR2" s="134"/>
-      <c r="AS2" s="135"/>
-      <c r="AT2" s="136" t="s">
+      <c r="AP2" s="136"/>
+      <c r="AQ2" s="136"/>
+      <c r="AR2" s="136"/>
+      <c r="AS2" s="137"/>
+      <c r="AT2" s="138" t="s">
         <v>12</v>
       </c>
-      <c r="AU2" s="137"/>
-      <c r="AV2" s="137"/>
-      <c r="AW2" s="137"/>
-      <c r="AX2" s="137"/>
-      <c r="AY2" s="138"/>
-      <c r="AZ2" s="133" t="s">
+      <c r="AU2" s="139"/>
+      <c r="AV2" s="139"/>
+      <c r="AW2" s="139"/>
+      <c r="AX2" s="139"/>
+      <c r="AY2" s="140"/>
+      <c r="AZ2" s="135" t="s">
         <v>12</v>
       </c>
-      <c r="BA2" s="134"/>
-      <c r="BB2" s="134"/>
-      <c r="BC2" s="134"/>
-      <c r="BD2" s="134"/>
-      <c r="BE2" s="135"/>
-      <c r="BF2" s="136" t="s">
+      <c r="BA2" s="136"/>
+      <c r="BB2" s="136"/>
+      <c r="BC2" s="136"/>
+      <c r="BD2" s="136"/>
+      <c r="BE2" s="137"/>
+      <c r="BF2" s="138" t="s">
         <v>12</v>
       </c>
-      <c r="BG2" s="137"/>
-      <c r="BH2" s="137"/>
-      <c r="BI2" s="137"/>
-      <c r="BJ2" s="137"/>
-      <c r="BK2" s="137"/>
-      <c r="BL2" s="138"/>
-      <c r="BM2" s="133" t="s">
+      <c r="BG2" s="139"/>
+      <c r="BH2" s="139"/>
+      <c r="BI2" s="139"/>
+      <c r="BJ2" s="139"/>
+      <c r="BK2" s="139"/>
+      <c r="BL2" s="140"/>
+      <c r="BM2" s="135" t="s">
         <v>12</v>
       </c>
-      <c r="BN2" s="134"/>
-      <c r="BO2" s="134"/>
-      <c r="BP2" s="134"/>
-      <c r="BQ2" s="134"/>
-      <c r="BR2" s="135"/>
-      <c r="BS2" s="136" t="s">
+      <c r="BN2" s="136"/>
+      <c r="BO2" s="136"/>
+      <c r="BP2" s="136"/>
+      <c r="BQ2" s="136"/>
+      <c r="BR2" s="137"/>
+      <c r="BS2" s="138" t="s">
         <v>12</v>
       </c>
-      <c r="BT2" s="137"/>
-      <c r="BU2" s="137"/>
-      <c r="BV2" s="137"/>
-      <c r="BW2" s="137"/>
-      <c r="BX2" s="138"/>
-      <c r="BY2" s="133" t="s">
+      <c r="BT2" s="139"/>
+      <c r="BU2" s="139"/>
+      <c r="BV2" s="139"/>
+      <c r="BW2" s="139"/>
+      <c r="BX2" s="140"/>
+      <c r="BY2" s="135" t="s">
         <v>12</v>
       </c>
-      <c r="BZ2" s="134"/>
-      <c r="CA2" s="134"/>
-      <c r="CB2" s="134"/>
-      <c r="CC2" s="135"/>
-      <c r="CD2" s="136" t="s">
+      <c r="BZ2" s="136"/>
+      <c r="CA2" s="136"/>
+      <c r="CB2" s="136"/>
+      <c r="CC2" s="137"/>
+      <c r="CD2" s="138" t="s">
         <v>12</v>
       </c>
-      <c r="CE2" s="137"/>
-      <c r="CF2" s="137"/>
-      <c r="CG2" s="137"/>
-      <c r="CH2" s="137"/>
-      <c r="CI2" s="138"/>
-      <c r="CJ2" s="133" t="s">
+      <c r="CE2" s="139"/>
+      <c r="CF2" s="139"/>
+      <c r="CG2" s="139"/>
+      <c r="CH2" s="139"/>
+      <c r="CI2" s="140"/>
+      <c r="CJ2" s="135" t="s">
         <v>12</v>
       </c>
-      <c r="CK2" s="134"/>
-      <c r="CL2" s="134"/>
-      <c r="CM2" s="134"/>
-      <c r="CN2" s="135"/>
-      <c r="CO2" s="136" t="s">
+      <c r="CK2" s="136"/>
+      <c r="CL2" s="136"/>
+      <c r="CM2" s="136"/>
+      <c r="CN2" s="137"/>
+      <c r="CO2" s="138" t="s">
         <v>12</v>
       </c>
-      <c r="CP2" s="137"/>
-      <c r="CQ2" s="137"/>
-      <c r="CR2" s="137"/>
-      <c r="CS2" s="138"/>
-      <c r="CT2" s="133" t="s">
+      <c r="CP2" s="139"/>
+      <c r="CQ2" s="139"/>
+      <c r="CR2" s="139"/>
+      <c r="CS2" s="140"/>
+      <c r="CT2" s="135" t="s">
         <v>12</v>
       </c>
-      <c r="CU2" s="134"/>
-      <c r="CV2" s="134"/>
-      <c r="CW2" s="134"/>
-      <c r="CX2" s="135"/>
-      <c r="CY2" s="136" t="s">
+      <c r="CU2" s="136"/>
+      <c r="CV2" s="136"/>
+      <c r="CW2" s="136"/>
+      <c r="CX2" s="137"/>
+      <c r="CY2" s="138" t="s">
         <v>12</v>
       </c>
-      <c r="CZ2" s="137"/>
-      <c r="DA2" s="137"/>
-      <c r="DB2" s="137"/>
-      <c r="DC2" s="137"/>
-      <c r="DD2" s="138"/>
-      <c r="DE2" s="133" t="s">
+      <c r="CZ2" s="139"/>
+      <c r="DA2" s="139"/>
+      <c r="DB2" s="139"/>
+      <c r="DC2" s="139"/>
+      <c r="DD2" s="140"/>
+      <c r="DE2" s="135" t="s">
         <v>12</v>
       </c>
-      <c r="DF2" s="134"/>
-      <c r="DG2" s="134"/>
-      <c r="DH2" s="134"/>
-      <c r="DI2" s="135"/>
-      <c r="DJ2" s="136" t="s">
+      <c r="DF2" s="136"/>
+      <c r="DG2" s="136"/>
+      <c r="DH2" s="136"/>
+      <c r="DI2" s="137"/>
+      <c r="DJ2" s="138" t="s">
         <v>12</v>
       </c>
-      <c r="DK2" s="137"/>
-      <c r="DL2" s="137"/>
-      <c r="DM2" s="137"/>
-      <c r="DN2" s="137"/>
-      <c r="DO2" s="138"/>
-      <c r="DP2" s="133" t="s">
+      <c r="DK2" s="139"/>
+      <c r="DL2" s="139"/>
+      <c r="DM2" s="139"/>
+      <c r="DN2" s="139"/>
+      <c r="DO2" s="140"/>
+      <c r="DP2" s="135" t="s">
         <v>12</v>
       </c>
-      <c r="DQ2" s="134"/>
-      <c r="DR2" s="134"/>
-      <c r="DS2" s="134"/>
-      <c r="DT2" s="134"/>
-      <c r="DU2" s="135"/>
-      <c r="DV2" s="136" t="s">
+      <c r="DQ2" s="136"/>
+      <c r="DR2" s="136"/>
+      <c r="DS2" s="136"/>
+      <c r="DT2" s="136"/>
+      <c r="DU2" s="137"/>
+      <c r="DV2" s="138" t="s">
         <v>12</v>
       </c>
-      <c r="DW2" s="137"/>
-      <c r="DX2" s="137"/>
-      <c r="DY2" s="137"/>
-      <c r="DZ2" s="138"/>
-      <c r="EA2" s="133" t="s">
+      <c r="DW2" s="139"/>
+      <c r="DX2" s="139"/>
+      <c r="DY2" s="139"/>
+      <c r="DZ2" s="140"/>
+      <c r="EA2" s="135" t="s">
         <v>12</v>
       </c>
-      <c r="EB2" s="134"/>
-      <c r="EC2" s="134"/>
-      <c r="ED2" s="134"/>
-      <c r="EE2" s="135"/>
-      <c r="EF2" s="136" t="s">
+      <c r="EB2" s="136"/>
+      <c r="EC2" s="136"/>
+      <c r="ED2" s="136"/>
+      <c r="EE2" s="137"/>
+      <c r="EF2" s="138" t="s">
         <v>12</v>
       </c>
-      <c r="EG2" s="137"/>
-      <c r="EH2" s="137"/>
-      <c r="EI2" s="137"/>
-      <c r="EJ2" s="137"/>
-      <c r="EK2" s="138"/>
-      <c r="EL2" s="133" t="s">
+      <c r="EG2" s="139"/>
+      <c r="EH2" s="139"/>
+      <c r="EI2" s="139"/>
+      <c r="EJ2" s="139"/>
+      <c r="EK2" s="140"/>
+      <c r="EL2" s="135" t="s">
         <v>12</v>
       </c>
-      <c r="EM2" s="134"/>
-      <c r="EN2" s="134"/>
-      <c r="EO2" s="134"/>
-      <c r="EP2" s="134"/>
-      <c r="EQ2" s="135"/>
-      <c r="ER2" s="136" t="s">
+      <c r="EM2" s="136"/>
+      <c r="EN2" s="136"/>
+      <c r="EO2" s="136"/>
+      <c r="EP2" s="136"/>
+      <c r="EQ2" s="137"/>
+      <c r="ER2" s="138" t="s">
         <v>12</v>
       </c>
-      <c r="ES2" s="137"/>
-      <c r="ET2" s="137"/>
-      <c r="EU2" s="137"/>
-      <c r="EV2" s="137"/>
-      <c r="EW2" s="138"/>
-      <c r="EX2" s="133" t="s">
+      <c r="ES2" s="139"/>
+      <c r="ET2" s="139"/>
+      <c r="EU2" s="139"/>
+      <c r="EV2" s="139"/>
+      <c r="EW2" s="140"/>
+      <c r="EX2" s="135" t="s">
         <v>12</v>
       </c>
-      <c r="EY2" s="134"/>
-      <c r="EZ2" s="134"/>
-      <c r="FA2" s="134"/>
-      <c r="FB2" s="134"/>
-      <c r="FC2" s="135"/>
-      <c r="FD2" s="136" t="s">
+      <c r="EY2" s="136"/>
+      <c r="EZ2" s="136"/>
+      <c r="FA2" s="136"/>
+      <c r="FB2" s="136"/>
+      <c r="FC2" s="137"/>
+      <c r="FD2" s="138" t="s">
         <v>12</v>
       </c>
-      <c r="FE2" s="137"/>
-      <c r="FF2" s="137"/>
-      <c r="FG2" s="137"/>
-      <c r="FH2" s="137"/>
-      <c r="FI2" s="138"/>
+      <c r="FE2" s="139"/>
+      <c r="FF2" s="139"/>
+      <c r="FG2" s="139"/>
+      <c r="FH2" s="139"/>
+      <c r="FI2" s="140"/>
     </row>
     <row r="3" spans="1:165" ht="15" x14ac:dyDescent="0.25">
       <c r="A3" s="15"/>
-      <c r="B3" s="131"/>
-      <c r="C3" s="125"/>
-      <c r="D3" s="125"/>
-      <c r="E3" s="125"/>
-      <c r="F3" s="125"/>
+      <c r="B3" s="133"/>
+      <c r="C3" s="124"/>
+      <c r="D3" s="124"/>
+      <c r="E3" s="124"/>
+      <c r="F3" s="124"/>
       <c r="G3" s="62">
         <v>2013</v>
       </c>
@@ -3010,11 +3054,11 @@
     </row>
     <row r="4" spans="1:165" ht="15" x14ac:dyDescent="0.25">
       <c r="A4" s="15"/>
-      <c r="B4" s="131"/>
-      <c r="C4" s="125"/>
-      <c r="D4" s="125"/>
-      <c r="E4" s="125"/>
-      <c r="F4" s="125"/>
+      <c r="B4" s="133"/>
+      <c r="C4" s="124"/>
+      <c r="D4" s="124"/>
+      <c r="E4" s="124"/>
+      <c r="F4" s="124"/>
       <c r="G4" s="69" t="s">
         <v>35</v>
       </c>
@@ -3495,11 +3539,11 @@
     </row>
     <row r="5" spans="1:165" ht="15" x14ac:dyDescent="0.25">
       <c r="A5" s="15"/>
-      <c r="B5" s="132"/>
-      <c r="C5" s="126"/>
-      <c r="D5" s="126"/>
-      <c r="E5" s="126"/>
-      <c r="F5" s="126"/>
+      <c r="B5" s="134"/>
+      <c r="C5" s="125"/>
+      <c r="D5" s="125"/>
+      <c r="E5" s="125"/>
+      <c r="F5" s="125"/>
       <c r="G5" s="78" t="s">
         <v>90</v>
       </c>
@@ -23681,13 +23725,13 @@
     <mergeCell ref="AD1:AI1"/>
     <mergeCell ref="BS1:BX1"/>
     <mergeCell ref="BM1:BR1"/>
+    <mergeCell ref="AZ1:BE1"/>
+    <mergeCell ref="BF1:BL1"/>
     <mergeCell ref="F2:F5"/>
     <mergeCell ref="B1:F1"/>
     <mergeCell ref="AJ1:AN1"/>
     <mergeCell ref="AO1:AS1"/>
     <mergeCell ref="AT1:AY1"/>
-    <mergeCell ref="AZ1:BE1"/>
-    <mergeCell ref="BF1:BL1"/>
     <mergeCell ref="C2:C5"/>
     <mergeCell ref="D2:D5"/>
     <mergeCell ref="E2:E5"/>
@@ -23704,4 +23748,62 @@
   <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
   <drawing r:id="rId1"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+  <dimension ref="A1:B7"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="33.85546875" customWidth="1"/>
+    <col min="2" max="2" width="18.140625" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1" s="121" t="s">
+        <v>123</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2" s="122" t="s">
+        <v>131</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A3" s="122" t="s">
+        <v>129</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A5" s="23" t="s">
+        <v>124</v>
+      </c>
+      <c r="B5" s="122" t="s">
+        <v>130</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A6" t="s">
+        <v>125</v>
+      </c>
+      <c r="B6" s="122" t="s">
+        <v>128</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A7" t="s">
+        <v>126</v>
+      </c>
+      <c r="B7" s="122" t="s">
+        <v>127</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.78740157499999996" bottom="0.78740157499999996" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>